<commit_message>
Finishing up the list
</commit_message>
<xml_diff>
--- a/dist/Allentown Pedigree.xlsx
+++ b/dist/Allentown Pedigree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\code\comic-book-pedigree-data\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945612FB-16DC-4C5B-BBBC-91213418956F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89BC1F0-9EE8-4142-AB15-1786A4AF347B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="101">
   <si>
     <t>All Winners</t>
   </si>
@@ -279,12 +279,6 @@
     <t>Issue</t>
   </si>
   <si>
-    <t>Estimated Grade</t>
-  </si>
-  <si>
-    <t>Estimated value</t>
-  </si>
-  <si>
     <t>Formerly an 8.0</t>
   </si>
   <si>
@@ -300,9 +294,6 @@
     <t>Highest graded is an 8.0</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>9 (c1)</t>
   </si>
   <si>
@@ -328,9 +319,6 @@
   </si>
   <si>
     <t>Best known copy</t>
-  </si>
-  <si>
-    <t>Listed as a #5 in the pedigree book sample chapter</t>
   </si>
   <si>
     <t>Not listed in pedigree book sample chapter</t>
@@ -363,7 +351,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -386,39 +374,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,47 +661,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I139"/>
+  <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I118" sqref="I118"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -755,17 +710,11 @@
       <c r="E2">
         <v>575</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H2" s="5">
-        <v>50000</v>
-      </c>
-      <c r="I2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -778,14 +727,8 @@
       <c r="E3">
         <v>6200</v>
       </c>
-      <c r="F3">
-        <v>7.5</v>
-      </c>
-      <c r="H3" s="5">
-        <v>750000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -798,14 +741,8 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="F4">
-        <v>8</v>
-      </c>
-      <c r="H4" s="5">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -818,14 +755,8 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="F5">
-        <v>9</v>
-      </c>
-      <c r="H5" s="5">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -838,14 +769,8 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="F6">
-        <v>9.6</v>
-      </c>
-      <c r="H6" s="5">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -858,14 +783,8 @@
       <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="F7">
-        <v>4.5</v>
-      </c>
-      <c r="H7" s="5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -878,17 +797,14 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <v>9.6</v>
       </c>
-      <c r="H8" s="5">
-        <v>50000</v>
-      </c>
-      <c r="I8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -901,14 +817,8 @@
       <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="F9">
-        <v>8.5</v>
-      </c>
-      <c r="H9" s="5">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -921,14 +831,8 @@
       <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="H10" s="5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -941,14 +845,8 @@
       <c r="D11" t="s">
         <v>39</v>
       </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -961,14 +859,8 @@
       <c r="D12" t="s">
         <v>39</v>
       </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
-      <c r="H12" s="5">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -984,14 +876,8 @@
       <c r="E13">
         <v>120</v>
       </c>
-      <c r="F13">
-        <v>9.6</v>
-      </c>
-      <c r="H13" s="5">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1007,17 +893,14 @@
       <c r="E14">
         <v>590</v>
       </c>
-      <c r="G14">
+      <c r="F14">
         <v>8</v>
       </c>
-      <c r="H14" s="5">
-        <v>2500</v>
-      </c>
-      <c r="I14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1033,17 +916,14 @@
       <c r="E15">
         <v>600</v>
       </c>
-      <c r="G15">
+      <c r="F15">
         <v>7</v>
       </c>
-      <c r="H15" s="5">
-        <v>3000</v>
-      </c>
-      <c r="I15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1059,14 +939,8 @@
       <c r="E16">
         <v>30</v>
       </c>
-      <c r="F16">
-        <v>6</v>
-      </c>
-      <c r="H16" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1082,14 +956,8 @@
       <c r="E17">
         <v>30</v>
       </c>
-      <c r="F17">
-        <v>7.5</v>
-      </c>
-      <c r="H17" s="5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1099,17 +967,14 @@
       <c r="C18" t="s">
         <v>3</v>
       </c>
-      <c r="G18">
+      <c r="F18">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H18" s="5">
-        <v>10000000</v>
-      </c>
-      <c r="I18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1122,14 +987,8 @@
       <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="F19">
-        <v>9.4</v>
-      </c>
-      <c r="H19" s="5">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1142,17 +1001,14 @@
       <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="G20">
+      <c r="F20">
         <v>9.6</v>
       </c>
-      <c r="H20" s="5">
-        <v>500000</v>
-      </c>
-      <c r="I20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1165,14 +1021,11 @@
       <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="G21">
+      <c r="F21">
         <v>8</v>
       </c>
-      <c r="H21" s="5">
-        <v>12500</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1185,14 +1038,8 @@
       <c r="D22" t="s">
         <v>39</v>
       </c>
-      <c r="F22">
-        <v>4.5</v>
-      </c>
-      <c r="H22" s="5">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1208,14 +1055,8 @@
       <c r="E23">
         <v>60</v>
       </c>
-      <c r="F23">
-        <v>8</v>
-      </c>
-      <c r="H23" s="5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1231,14 +1072,8 @@
       <c r="E24">
         <v>15</v>
       </c>
-      <c r="F24">
-        <v>2.5</v>
-      </c>
-      <c r="H24" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1254,14 +1089,8 @@
       <c r="E25">
         <v>1400</v>
       </c>
-      <c r="F25">
-        <v>9.4</v>
-      </c>
-      <c r="H25" s="5">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1277,14 +1106,8 @@
       <c r="E26">
         <v>500</v>
       </c>
-      <c r="F26">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="H26" s="5">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1297,17 +1120,11 @@
       <c r="D27" t="s">
         <v>15</v>
       </c>
-      <c r="F27">
-        <v>9.4</v>
-      </c>
-      <c r="H27" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1320,17 +1137,11 @@
       <c r="D28" t="s">
         <v>15</v>
       </c>
-      <c r="F28">
-        <v>9.4</v>
-      </c>
-      <c r="H28" s="5">
-        <v>22500000</v>
-      </c>
-      <c r="I28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1343,14 +1154,8 @@
       <c r="D29" t="s">
         <v>15</v>
       </c>
-      <c r="F29">
-        <v>9</v>
-      </c>
-      <c r="H29" s="5">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1363,17 +1168,14 @@
       <c r="D30" t="s">
         <v>15</v>
       </c>
-      <c r="G30">
+      <c r="F30">
         <v>9.6</v>
       </c>
-      <c r="H30" s="5">
-        <v>1500000</v>
-      </c>
-      <c r="I30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1386,14 +1188,8 @@
       <c r="D31" t="s">
         <v>17</v>
       </c>
-      <c r="F31">
-        <v>9</v>
-      </c>
-      <c r="H31" s="5">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1409,17 +1205,11 @@
       <c r="E32">
         <v>2300</v>
       </c>
-      <c r="F32">
-        <v>9</v>
-      </c>
-      <c r="H32" s="5">
-        <v>1500000</v>
-      </c>
-      <c r="I32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1432,14 +1222,11 @@
       <c r="D33" t="s">
         <v>15</v>
       </c>
-      <c r="G33">
+      <c r="F33">
         <v>9</v>
       </c>
-      <c r="H33" s="5">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1452,14 +1239,8 @@
       <c r="D34" t="s">
         <v>15</v>
       </c>
-      <c r="F34">
-        <v>9</v>
-      </c>
-      <c r="H34" s="5">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1472,14 +1253,8 @@
       <c r="D35" t="s">
         <v>15</v>
       </c>
-      <c r="F35">
-        <v>9</v>
-      </c>
-      <c r="H35" s="5">
-        <v>250000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1492,17 +1267,14 @@
       <c r="D36" t="s">
         <v>15</v>
       </c>
-      <c r="G36">
+      <c r="F36">
         <v>9.4</v>
       </c>
-      <c r="H36" s="5">
-        <v>1000000</v>
-      </c>
-      <c r="I36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1515,14 +1287,8 @@
       <c r="D37" t="s">
         <v>15</v>
       </c>
-      <c r="F37">
-        <v>9.6</v>
-      </c>
-      <c r="H37" s="5">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1535,14 +1301,8 @@
       <c r="D38" t="s">
         <v>15</v>
       </c>
-      <c r="F38">
-        <v>9.4</v>
-      </c>
-      <c r="H38" s="5">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1555,14 +1315,8 @@
       <c r="D39" t="s">
         <v>15</v>
       </c>
-      <c r="F39">
-        <v>9.4</v>
-      </c>
-      <c r="H39" s="5">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1575,14 +1329,8 @@
       <c r="D40" t="s">
         <v>9</v>
       </c>
-      <c r="F40">
-        <v>6</v>
-      </c>
-      <c r="H40" s="5">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -1598,14 +1346,8 @@
       <c r="E41">
         <v>120</v>
       </c>
-      <c r="F41">
-        <v>8</v>
-      </c>
-      <c r="H41" s="5">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1621,14 +1363,8 @@
       <c r="E42">
         <v>85</v>
       </c>
-      <c r="F42">
-        <v>9</v>
-      </c>
-      <c r="H42" s="5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -1644,14 +1380,11 @@
       <c r="E43">
         <v>85</v>
       </c>
-      <c r="G43">
+      <c r="F43">
         <v>9.4</v>
       </c>
-      <c r="H43" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -1667,14 +1400,8 @@
       <c r="E44">
         <v>95</v>
       </c>
-      <c r="F44">
-        <v>8</v>
-      </c>
-      <c r="H44" s="5">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1690,31 +1417,22 @@
       <c r="E45">
         <v>80</v>
       </c>
-      <c r="F45">
-        <v>8</v>
-      </c>
-      <c r="H45" s="5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>21</v>
       </c>
       <c r="B46">
         <v>22</v>
       </c>
-      <c r="G46">
+      <c r="F46">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H46" s="5">
-        <v>1000</v>
-      </c>
-      <c r="I46" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -1730,14 +1448,8 @@
       <c r="E47">
         <v>420</v>
       </c>
-      <c r="F47">
-        <v>8</v>
-      </c>
-      <c r="H47" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -1754,21 +1466,15 @@
         <v>70</v>
       </c>
       <c r="F48">
-        <v>7.5</v>
-      </c>
-      <c r="G48">
         <v>7</v>
       </c>
-      <c r="H48" s="5">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C49" t="s">
         <v>26</v>
@@ -1779,14 +1485,8 @@
       <c r="E49">
         <v>40</v>
       </c>
-      <c r="F49">
-        <v>6</v>
-      </c>
-      <c r="H49" s="5">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>27</v>
       </c>
@@ -1803,16 +1503,10 @@
         <v>28</v>
       </c>
       <c r="F50">
-        <v>9</v>
-      </c>
-      <c r="G50">
         <v>9.4</v>
       </c>
-      <c r="H50" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -1825,14 +1519,11 @@
       <c r="E51">
         <v>18000</v>
       </c>
-      <c r="G51" t="s">
+      <c r="F51" t="s">
         <v>76</v>
       </c>
-      <c r="H51" s="5">
-        <v>250000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -1848,14 +1539,8 @@
       <c r="E52">
         <v>695</v>
       </c>
-      <c r="F52">
-        <v>9</v>
-      </c>
-      <c r="H52" s="5">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -1868,17 +1553,14 @@
       <c r="D53" t="s">
         <v>15</v>
       </c>
-      <c r="G53">
+      <c r="F53">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H53" s="5">
-        <v>200000</v>
-      </c>
-      <c r="I53" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -1891,17 +1573,11 @@
       <c r="D54" t="s">
         <v>15</v>
       </c>
-      <c r="F54">
-        <v>9.6</v>
-      </c>
-      <c r="H54" s="5">
-        <v>50000</v>
-      </c>
-      <c r="I54" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -1914,14 +1590,8 @@
       <c r="D55" t="s">
         <v>15</v>
       </c>
-      <c r="F55">
-        <v>9.6</v>
-      </c>
-      <c r="H55" s="5">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -1934,14 +1604,8 @@
       <c r="D56" t="s">
         <v>15</v>
       </c>
-      <c r="F56">
-        <v>9.6</v>
-      </c>
-      <c r="H56" s="5">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -1954,14 +1618,8 @@
       <c r="D57" t="s">
         <v>15</v>
       </c>
-      <c r="F57">
-        <v>9.4</v>
-      </c>
-      <c r="H57" s="5">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -1974,14 +1632,8 @@
       <c r="D58" t="s">
         <v>15</v>
       </c>
-      <c r="F58">
-        <v>9.4</v>
-      </c>
-      <c r="H58" s="5">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>43</v>
       </c>
@@ -1994,14 +1646,8 @@
       <c r="D59" t="s">
         <v>6</v>
       </c>
-      <c r="F59">
-        <v>7</v>
-      </c>
-      <c r="H59" s="5">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -2014,14 +1660,8 @@
       <c r="D60" t="s">
         <v>15</v>
       </c>
-      <c r="F60">
-        <v>9.4</v>
-      </c>
-      <c r="H60" s="5">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -2034,14 +1674,8 @@
       <c r="D61" t="s">
         <v>15</v>
       </c>
-      <c r="F61">
-        <v>9.4</v>
-      </c>
-      <c r="H61" s="5">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -2054,14 +1688,8 @@
       <c r="D62" t="s">
         <v>15</v>
       </c>
-      <c r="F62">
-        <v>9</v>
-      </c>
-      <c r="H62" s="5">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -2071,14 +1699,11 @@
       <c r="C63" t="s">
         <v>17</v>
       </c>
-      <c r="G63">
+      <c r="F63">
         <v>9</v>
       </c>
-      <c r="H63" s="5">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>43</v>
       </c>
@@ -2091,17 +1716,14 @@
       <c r="D64" t="s">
         <v>15</v>
       </c>
-      <c r="G64">
+      <c r="F64">
         <v>9.6</v>
       </c>
-      <c r="H64" s="5">
-        <v>25000</v>
-      </c>
-      <c r="I64" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -2114,14 +1736,11 @@
       <c r="D65" t="s">
         <v>15</v>
       </c>
-      <c r="G65">
+      <c r="F65">
         <v>9</v>
       </c>
-      <c r="H65" s="5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -2134,14 +1753,8 @@
       <c r="D66" t="s">
         <v>4</v>
       </c>
-      <c r="F66">
-        <v>8.5</v>
-      </c>
-      <c r="H66" s="5">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -2154,14 +1767,8 @@
       <c r="D67" t="s">
         <v>15</v>
       </c>
-      <c r="F67">
-        <v>9</v>
-      </c>
-      <c r="H67" s="5">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>32</v>
       </c>
@@ -2177,14 +1784,11 @@
       <c r="E68">
         <v>2300</v>
       </c>
-      <c r="G68">
+      <c r="F68">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H68" s="5">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>32</v>
       </c>
@@ -2200,20 +1804,14 @@
       <c r="E69">
         <v>800</v>
       </c>
-      <c r="F69" t="s">
-        <v>91</v>
-      </c>
-      <c r="G69">
+      <c r="F69">
         <v>9.4</v>
       </c>
-      <c r="H69" s="5">
-        <v>60000</v>
-      </c>
-      <c r="I69" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G69" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>32</v>
       </c>
@@ -2229,17 +1827,14 @@
       <c r="E70">
         <v>695</v>
       </c>
-      <c r="G70">
+      <c r="F70">
         <v>9.4</v>
       </c>
-      <c r="H70" s="5">
-        <v>40000</v>
-      </c>
-      <c r="I70" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G70" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -2255,14 +1850,8 @@
       <c r="E71">
         <v>200</v>
       </c>
-      <c r="F71">
-        <v>5</v>
-      </c>
-      <c r="H71" s="4">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -2278,14 +1867,8 @@
       <c r="E72">
         <v>280</v>
       </c>
-      <c r="F72">
-        <v>9.6</v>
-      </c>
-      <c r="H72" s="5">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>33</v>
       </c>
@@ -2301,14 +1884,8 @@
       <c r="E73">
         <v>240</v>
       </c>
-      <c r="F73">
-        <v>9.6</v>
-      </c>
-      <c r="H73" s="5">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>33</v>
       </c>
@@ -2324,14 +1901,8 @@
       <c r="E74">
         <v>200</v>
       </c>
-      <c r="F74">
-        <v>9.6</v>
-      </c>
-      <c r="H74" s="5">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>33</v>
       </c>
@@ -2347,31 +1918,22 @@
       <c r="E75">
         <v>130</v>
       </c>
-      <c r="F75">
-        <v>8</v>
-      </c>
-      <c r="G75" t="s">
-        <v>92</v>
-      </c>
-      <c r="H75" s="5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>33</v>
       </c>
       <c r="B76">
         <v>7</v>
       </c>
-      <c r="G76">
+      <c r="F76">
         <v>6.5</v>
       </c>
-      <c r="H76" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>33</v>
       </c>
@@ -2384,14 +1946,11 @@
       <c r="D77" t="s">
         <v>15</v>
       </c>
-      <c r="G77">
+      <c r="F77">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H77" s="5">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -2407,14 +1966,8 @@
       <c r="E78">
         <v>215</v>
       </c>
-      <c r="F78">
-        <v>9.4</v>
-      </c>
-      <c r="H78" s="5">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -2430,11 +1983,8 @@
       <c r="F79">
         <v>9.4</v>
       </c>
-      <c r="H79" s="5">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -2447,14 +1997,8 @@
       <c r="E80">
         <v>200</v>
       </c>
-      <c r="F80">
-        <v>8</v>
-      </c>
-      <c r="H80" s="5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -2467,14 +2011,8 @@
       <c r="E81">
         <v>225</v>
       </c>
-      <c r="F81">
-        <v>9</v>
-      </c>
-      <c r="H81" s="5">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>49</v>
       </c>
@@ -2487,14 +2025,11 @@
       <c r="E82">
         <v>230</v>
       </c>
-      <c r="G82">
+      <c r="F82">
         <v>9</v>
       </c>
-      <c r="H82" s="5">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>50</v>
       </c>
@@ -2507,14 +2042,8 @@
       <c r="E83">
         <v>190</v>
       </c>
-      <c r="F83">
-        <v>6</v>
-      </c>
-      <c r="H83" s="5">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>52</v>
       </c>
@@ -2527,11 +2056,8 @@
       <c r="E84">
         <v>20</v>
       </c>
-      <c r="F84">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>54</v>
       </c>
@@ -2547,14 +2073,8 @@
       <c r="E85">
         <v>45</v>
       </c>
-      <c r="F85">
-        <v>8</v>
-      </c>
-      <c r="H85" s="5">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>54</v>
       </c>
@@ -2570,14 +2090,8 @@
       <c r="E86">
         <v>13</v>
       </c>
-      <c r="F86">
-        <v>8</v>
-      </c>
-      <c r="H86" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>55</v>
       </c>
@@ -2593,14 +2107,8 @@
       <c r="E87">
         <v>210</v>
       </c>
-      <c r="F87">
-        <v>8</v>
-      </c>
-      <c r="H87" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>56</v>
       </c>
@@ -2616,14 +2124,8 @@
       <c r="E88">
         <v>180</v>
       </c>
-      <c r="F88">
-        <v>8</v>
-      </c>
-      <c r="H88" s="5">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>56</v>
       </c>
@@ -2639,14 +2141,8 @@
       <c r="E89">
         <v>170</v>
       </c>
-      <c r="F89">
-        <v>8</v>
-      </c>
-      <c r="H89" s="5">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>57</v>
       </c>
@@ -2662,17 +2158,14 @@
       <c r="E90">
         <v>1600</v>
       </c>
-      <c r="G90">
+      <c r="F90">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H90" s="5">
-        <v>250000</v>
-      </c>
-      <c r="I90" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G90" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>58</v>
       </c>
@@ -2688,17 +2181,14 @@
       <c r="E91">
         <v>1800</v>
       </c>
-      <c r="G91">
+      <c r="F91">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H91" s="5">
-        <v>75000</v>
-      </c>
-      <c r="I91" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G91" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>59</v>
       </c>
@@ -2714,14 +2204,8 @@
       <c r="E92">
         <v>425</v>
       </c>
-      <c r="F92">
-        <v>9.4</v>
-      </c>
-      <c r="H92" s="5">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>59</v>
       </c>
@@ -2737,17 +2221,11 @@
       <c r="E93">
         <v>125</v>
       </c>
-      <c r="F93">
-        <v>9.4</v>
-      </c>
-      <c r="H93" s="5">
-        <v>20000</v>
-      </c>
-      <c r="I93" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>60</v>
       </c>
@@ -2763,14 +2241,11 @@
       <c r="E94">
         <v>230</v>
       </c>
-      <c r="G94">
+      <c r="F94">
         <v>7</v>
       </c>
-      <c r="H94" s="5">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>61</v>
       </c>
@@ -2786,14 +2261,8 @@
       <c r="E95">
         <v>135</v>
       </c>
-      <c r="F95">
-        <v>9.4</v>
-      </c>
-      <c r="H95" s="5">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>61</v>
       </c>
@@ -2809,14 +2278,8 @@
       <c r="E96">
         <v>10</v>
       </c>
-      <c r="F96">
-        <v>3</v>
-      </c>
-      <c r="H96" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>61</v>
       </c>
@@ -2832,14 +2295,8 @@
       <c r="E97">
         <v>20</v>
       </c>
-      <c r="F97">
-        <v>4</v>
-      </c>
-      <c r="H97" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>64</v>
       </c>
@@ -2855,14 +2312,8 @@
       <c r="E98">
         <v>325</v>
       </c>
-      <c r="F98">
-        <v>8</v>
-      </c>
-      <c r="H98" s="5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>65</v>
       </c>
@@ -2878,14 +2329,8 @@
       <c r="E99">
         <v>240</v>
       </c>
-      <c r="F99">
-        <v>8</v>
-      </c>
-      <c r="H99" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>65</v>
       </c>
@@ -2901,11 +2346,11 @@
       <c r="E100">
         <v>150</v>
       </c>
-      <c r="H100" s="5">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F100">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>65</v>
       </c>
@@ -2921,14 +2366,11 @@
       <c r="E101">
         <v>120</v>
       </c>
-      <c r="G101">
+      <c r="F101">
         <v>7.5</v>
       </c>
-      <c r="H101" s="5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>66</v>
       </c>
@@ -2944,14 +2386,8 @@
       <c r="E102">
         <v>20</v>
       </c>
-      <c r="F102">
-        <v>2</v>
-      </c>
-      <c r="H102" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>68</v>
       </c>
@@ -2967,14 +2403,11 @@
       <c r="E103">
         <v>90</v>
       </c>
-      <c r="G103">
+      <c r="F103">
         <v>9</v>
       </c>
-      <c r="H103" s="5">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>68</v>
       </c>
@@ -2990,14 +2423,8 @@
       <c r="E104">
         <v>145</v>
       </c>
-      <c r="F104">
-        <v>9.4</v>
-      </c>
-      <c r="H104" s="5">
-        <v>12500</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>69</v>
       </c>
@@ -3013,14 +2440,8 @@
       <c r="E105">
         <v>20</v>
       </c>
-      <c r="F105">
-        <v>9.4</v>
-      </c>
-      <c r="H105" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>70</v>
       </c>
@@ -3036,14 +2457,8 @@
       <c r="E106">
         <v>17</v>
       </c>
-      <c r="F106">
-        <v>6</v>
-      </c>
-      <c r="H106" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>70</v>
       </c>
@@ -3059,14 +2474,8 @@
       <c r="E107">
         <v>17</v>
       </c>
-      <c r="F107">
-        <v>8</v>
-      </c>
-      <c r="H107" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>71</v>
       </c>
@@ -3076,14 +2485,8 @@
       <c r="D108" t="s">
         <v>15</v>
       </c>
-      <c r="F108">
-        <v>9.6</v>
-      </c>
-      <c r="H108" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>72</v>
       </c>
@@ -3099,14 +2502,8 @@
       <c r="E109">
         <v>40</v>
       </c>
-      <c r="F109">
-        <v>9.4</v>
-      </c>
-      <c r="H109" s="5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>72</v>
       </c>
@@ -3122,14 +2519,11 @@
       <c r="E110">
         <v>18</v>
       </c>
-      <c r="G110">
+      <c r="F110">
         <v>9</v>
       </c>
-      <c r="H110" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>72</v>
       </c>
@@ -3145,14 +2539,8 @@
       <c r="E111">
         <v>47</v>
       </c>
-      <c r="F111">
-        <v>9.4</v>
-      </c>
-      <c r="H111" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>72</v>
       </c>
@@ -3168,14 +2556,8 @@
       <c r="E112">
         <v>5</v>
       </c>
-      <c r="F112">
-        <v>6</v>
-      </c>
-      <c r="H112" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>73</v>
       </c>
@@ -3191,17 +2573,14 @@
       <c r="E113">
         <v>540</v>
       </c>
-      <c r="G113">
+      <c r="F113">
         <v>9.6</v>
       </c>
-      <c r="H113" s="5">
-        <v>25000</v>
-      </c>
-      <c r="I113" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G113" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>73</v>
       </c>
@@ -3217,17 +2596,14 @@
       <c r="E114">
         <v>475</v>
       </c>
-      <c r="G114">
+      <c r="F114">
         <v>8.5</v>
       </c>
-      <c r="H114" s="5">
-        <v>15000</v>
-      </c>
-      <c r="I114" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G114" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>44</v>
       </c>
@@ -3240,14 +2616,11 @@
       <c r="D115" t="s">
         <v>15</v>
       </c>
-      <c r="G115">
+      <c r="F115">
         <v>9.4</v>
       </c>
-      <c r="H115" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>44</v>
       </c>
@@ -3260,31 +2633,22 @@
       <c r="D116" t="s">
         <v>15</v>
       </c>
-      <c r="F116">
-        <v>9.4</v>
-      </c>
-      <c r="H116" s="5">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>44</v>
       </c>
       <c r="B117">
         <v>5</v>
       </c>
-      <c r="G117">
+      <c r="F117">
         <v>9.4</v>
       </c>
-      <c r="H117" s="5">
-        <v>2500</v>
-      </c>
-      <c r="I117" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G117" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>44</v>
       </c>
@@ -3297,14 +2661,8 @@
       <c r="D118" t="s">
         <v>17</v>
       </c>
-      <c r="F118">
-        <v>8</v>
-      </c>
-      <c r="H118" s="5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>44</v>
       </c>
@@ -3317,14 +2675,8 @@
       <c r="D119" t="s">
         <v>15</v>
       </c>
-      <c r="F119">
-        <v>8</v>
-      </c>
-      <c r="H119" s="5">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>44</v>
       </c>
@@ -3337,17 +2689,14 @@
       <c r="D120" t="s">
         <v>15</v>
       </c>
-      <c r="G120">
+      <c r="F120">
         <v>9.4</v>
       </c>
-      <c r="H120" s="5">
-        <v>1200</v>
-      </c>
-      <c r="I120" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G120" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>44</v>
       </c>
@@ -3360,14 +2709,8 @@
       <c r="D121" t="s">
         <v>15</v>
       </c>
-      <c r="F121">
-        <v>8</v>
-      </c>
-      <c r="H121" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>44</v>
       </c>
@@ -3380,14 +2723,8 @@
       <c r="D122" t="s">
         <v>15</v>
       </c>
-      <c r="F122">
-        <v>8</v>
-      </c>
-      <c r="H122" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>45</v>
       </c>
@@ -3403,14 +2740,11 @@
       <c r="E123">
         <v>1960</v>
       </c>
-      <c r="G123" t="s">
+      <c r="F123" t="s">
         <v>75</v>
       </c>
-      <c r="H123" s="5">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>45</v>
       </c>
@@ -3426,14 +2760,11 @@
       <c r="E124">
         <v>1000</v>
       </c>
-      <c r="G124">
+      <c r="F124">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H124" s="5">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>46</v>
       </c>
@@ -3446,14 +2777,11 @@
       <c r="D125" t="s">
         <v>15</v>
       </c>
-      <c r="G125">
+      <c r="F125">
         <v>9.4</v>
       </c>
-      <c r="H125" s="5">
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>46</v>
       </c>
@@ -3466,14 +2794,8 @@
       <c r="D126" t="s">
         <v>15</v>
       </c>
-      <c r="F126">
-        <v>8</v>
-      </c>
-      <c r="H126" s="5">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>46</v>
       </c>
@@ -3486,17 +2808,11 @@
       <c r="D127" t="s">
         <v>15</v>
       </c>
-      <c r="F127">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="H127" s="5">
-        <v>10000</v>
-      </c>
-      <c r="I127" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G127" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>46</v>
       </c>
@@ -3510,13 +2826,13 @@
         <v>15</v>
       </c>
       <c r="F128">
-        <v>9</v>
-      </c>
-      <c r="H128" s="5">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G128" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>46</v>
       </c>
@@ -3529,14 +2845,8 @@
       <c r="D129" t="s">
         <v>15</v>
       </c>
-      <c r="F129">
-        <v>9</v>
-      </c>
-      <c r="H129" s="5">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>46</v>
       </c>
@@ -3549,17 +2859,14 @@
       <c r="D130" t="s">
         <v>15</v>
       </c>
-      <c r="G130">
+      <c r="F130">
         <v>9.4</v>
       </c>
-      <c r="H130" s="5">
-        <v>50000</v>
-      </c>
-      <c r="I130" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G130" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>46</v>
       </c>
@@ -3572,17 +2879,11 @@
       <c r="D131" t="s">
         <v>15</v>
       </c>
-      <c r="F131">
-        <v>9</v>
-      </c>
-      <c r="H131" s="5">
-        <v>25000</v>
-      </c>
-      <c r="I131" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G131" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>46</v>
       </c>
@@ -3595,17 +2896,14 @@
       <c r="D132" t="s">
         <v>15</v>
       </c>
-      <c r="G132">
+      <c r="F132">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H132" s="5">
-        <v>25000</v>
-      </c>
-      <c r="I132" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G132" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>46</v>
       </c>
@@ -3621,14 +2919,8 @@
       <c r="E133">
         <v>270</v>
       </c>
-      <c r="F133">
-        <v>6</v>
-      </c>
-      <c r="H133" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>46</v>
       </c>
@@ -3641,14 +2933,8 @@
       <c r="D134" t="s">
         <v>15</v>
       </c>
-      <c r="F134">
-        <v>9</v>
-      </c>
-      <c r="H134" s="5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>46</v>
       </c>
@@ -3661,17 +2947,14 @@
       <c r="D135" t="s">
         <v>15</v>
       </c>
-      <c r="G135">
+      <c r="F135">
         <v>9.6</v>
       </c>
-      <c r="H135" s="5">
-        <v>40000</v>
-      </c>
-      <c r="I135" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G135" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>46</v>
       </c>
@@ -3684,17 +2967,11 @@
       <c r="D136" t="s">
         <v>15</v>
       </c>
-      <c r="F136" t="s">
-        <v>91</v>
-      </c>
-      <c r="G136">
+      <c r="F136">
         <v>8</v>
       </c>
-      <c r="H136" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>46</v>
       </c>
@@ -3707,17 +2984,11 @@
       <c r="D137" t="s">
         <v>15</v>
       </c>
-      <c r="F137">
-        <v>9.4</v>
-      </c>
-      <c r="H137" s="5">
-        <v>50000</v>
-      </c>
-      <c r="I137" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G137" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>46</v>
       </c>
@@ -3733,14 +3004,8 @@
       <c r="E138">
         <v>78</v>
       </c>
-      <c r="F138">
-        <v>7</v>
-      </c>
-      <c r="H138" s="5">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>74</v>
       </c>
@@ -3757,10 +3022,7 @@
         <v>150</v>
       </c>
       <c r="F139">
-        <v>9.4</v>
-      </c>
-      <c r="H139" s="5">
-        <v>25000</v>
+        <v>9.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>